<commit_message>
Adding excel files and creating get available usd
</commit_message>
<xml_diff>
--- a/src/kraken_files/excel_files/AAVEUSD.xlsx
+++ b/src/kraken_files/excel_files/AAVEUSD.xlsx
@@ -484,16 +484,16 @@
         <v>0.3125</v>
       </c>
       <c r="D2" t="n">
-        <v>295.19602507776</v>
+        <v>304.71762034176</v>
       </c>
       <c r="E2" t="n">
-        <v>306.90111996288</v>
+        <v>316.80026494488</v>
       </c>
       <c r="F2" t="n">
-        <v>309.9701311625088</v>
+        <v>319.9682675943288</v>
       </c>
       <c r="G2" t="n">
-        <v>4.766299910684979</v>
+        <v>4.766299910684991</v>
       </c>
     </row>
     <row r="3">
@@ -507,16 +507,16 @@
         <v>0.78125</v>
       </c>
       <c r="D3" t="n">
-        <v>269.53635911464</v>
+        <v>278.230297726265</v>
       </c>
       <c r="E3" t="n">
-        <v>288.21873953876</v>
+        <v>297.5152813355725</v>
       </c>
       <c r="F3" t="n">
-        <v>291.1009269341476</v>
+        <v>300.4904341489282</v>
       </c>
       <c r="G3" t="n">
-        <v>7.407935126357712</v>
+        <v>7.407935126357701</v>
       </c>
     </row>
     <row r="4">
@@ -530,16 +530,16 @@
         <v>1.953125</v>
       </c>
       <c r="D4" t="n">
-        <v>229.507280225504</v>
+        <v>236.910074459854</v>
       </c>
       <c r="E4" t="n">
-        <v>258.863009882132</v>
+        <v>267.2126778977132</v>
       </c>
       <c r="F4" t="n">
-        <v>261.4516399809534</v>
+        <v>269.8848046766904</v>
       </c>
       <c r="G4" t="n">
-        <v>12.21807587735022</v>
+        <v>12.21807587735019</v>
       </c>
     </row>
     <row r="5">
@@ -553,16 +553,16 @@
         <v>4.8828125</v>
       </c>
       <c r="D5" t="n">
-        <v>167.06191714912</v>
+        <v>172.45052615462</v>
       </c>
       <c r="E5" t="n">
-        <v>212.962463515626</v>
+        <v>219.8316020261666</v>
       </c>
       <c r="F5" t="n">
-        <v>215.0920881507822</v>
+        <v>222.0299180464283</v>
       </c>
       <c r="G5" t="n">
-        <v>22.33005007975585</v>
+        <v>22.33005007975584</v>
       </c>
     </row>
   </sheetData>
@@ -576,7 +576,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -599,21 +599,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>OTAJM3-VPCAK-JANKD6</t>
+          <t>O736YO-27F72-JGBIPY</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>328.82</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>OOA6WP-64JU5-6KOYXS</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>321.79</v>
+        <v>332.17</v>
       </c>
     </row>
   </sheetData>
@@ -627,7 +617,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -645,14 +635,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>OEQ5T6-HNQCU-WKMJYJ</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>OJG3BE-436LG-CLB5NB</t>
+          <t>OGI3BN-DA3HY-C25WXB</t>
         </is>
       </c>
     </row>

</xml_diff>